<commit_message>
Exel file update, testbilder update
</commit_message>
<xml_diff>
--- a/code/testset/image_numbers.xlsx
+++ b/code/testset/image_numbers.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="228" yWindow="576" windowWidth="13116" windowHeight="3396"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tabelle1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Tabelle2" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Tabelle3" sheetId="3" r:id="rId5"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Math- Solver</t>
   </si>
@@ -205,31 +208,102 @@
   </si>
   <si>
     <t>86*73*11*58*21*19</t>
+  </si>
+  <si>
+    <t>(13+11)/2</t>
+  </si>
+  <si>
+    <t>(14*3)-1</t>
+  </si>
+  <si>
+    <t>((7+4)*30)/4</t>
+  </si>
+  <si>
+    <t>500-40</t>
+  </si>
+  <si>
+    <t>1337-27</t>
+  </si>
+  <si>
+    <t>(42+34)*9</t>
+  </si>
+  <si>
+    <t>(47*11)/(4-2)</t>
+  </si>
+  <si>
+    <t>(0-9)/(-7)</t>
+  </si>
+  <si>
+    <t>((679+1)/2)*4</t>
+  </si>
+  <si>
+    <t>(49+7-4)*5</t>
+  </si>
+  <si>
+    <t>717+471/-7</t>
+  </si>
+  <si>
+    <t>874+37*111</t>
+  </si>
+  <si>
+    <t>(69+69)*71</t>
+  </si>
+  <si>
+    <t>666-111*3</t>
+  </si>
+  <si>
+    <t>(1995-21)*3</t>
+  </si>
+  <si>
+    <t>(50/5)*(5-4)</t>
+  </si>
+  <si>
+    <t>(612-4+7)/2</t>
+  </si>
+  <si>
+    <t>46-0+8</t>
+  </si>
+  <si>
+    <t>8+8</t>
+  </si>
+  <si>
+    <t>7-7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,79 +311,379 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+  <a:themeElements>
+    <a:clrScheme name="Larissa">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Larissa">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Larissa">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.63"/>
-    <col customWidth="1" min="2" max="2" width="21.25"/>
-    <col customWidth="1" min="3" max="26" width="9.38"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="26" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:4" ht="14.25" customHeight="1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -320,45 +694,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:4" ht="14.25" customHeight="1">
       <c r="A3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:4" ht="14.25" customHeight="1">
       <c r="A4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3">
-        <v>282.0</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>2054.66667</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
+        <v>2054.6666700000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.25" customHeight="1">
       <c r="A6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -367,86 +741,86 @@
         <v>5040.04</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:4" ht="14.25" customHeight="1">
       <c r="A7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1">
       <c r="A8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="3">
-        <v>67497.1316</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1">
+        <v>67497.131599999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1">
       <c r="A9">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="3">
-        <v>139.0</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1">
       <c r="A10">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="3">
-        <v>1426.0</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25" customHeight="1">
       <c r="A11">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="3">
-        <v>2014.0</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.25" customHeight="1">
       <c r="A12">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3">
-        <v>4814.14957</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
+        <v>4814.1495699999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.25" customHeight="1">
       <c r="A13">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="3">
-        <v>1445.0</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1">
       <c r="A14">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -455,53 +829,53 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:4" ht="14.25" customHeight="1">
       <c r="A15">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="3">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.25" customHeight="1">
       <c r="A16">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="3">
-        <v>49.0</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3">
-        <v>3232.0</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="3">
-        <v>959.0</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>21</v>
@@ -510,384 +884,504 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="3">
-        <v>44.0</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="3">
-        <v>7.42857143</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
+        <v>7.4285714299999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="3">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="2">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="2">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="2">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="2">
-        <v>139.0</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="2">
-        <v>256.0</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="2">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="2">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="2">
-        <v>180.0</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="2">
-        <v>419.0</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="2">
-        <v>42.0</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="2">
-        <v>31.0</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="2">
-        <v>215.0</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="2">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C37" s="2">
-        <v>-267.0</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
+        <v>-267</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C38" s="2">
-        <v>255.0</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C39" s="2">
-        <v>864.0</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="2">
-        <v>65.0</v>
-      </c>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="2">
-        <v>1443.0</v>
-      </c>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
       <c r="A42">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C42" s="2">
-        <v>41.0</v>
-      </c>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43">
-        <v>40.0</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44">
-        <v>41.0</v>
-      </c>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45">
-        <v>42.0</v>
-      </c>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="A46">
-        <v>43.0</v>
-      </c>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="A47">
-        <v>44.0</v>
-      </c>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48">
-        <v>45.0</v>
-      </c>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49">
-        <v>46.0</v>
-      </c>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50">
-        <v>47.0</v>
-      </c>
-    </row>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="A51">
-        <v>48.0</v>
-      </c>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="A52">
-        <v>49.0</v>
-      </c>
-    </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="54" ht="14.25" customHeight="1">
-      <c r="A54">
-        <v>51.0</v>
-      </c>
-    </row>
-    <row r="55" ht="14.25" customHeight="1">
-      <c r="A55">
-        <v>52.0</v>
-      </c>
-    </row>
-    <row r="56" ht="14.25" customHeight="1">
-      <c r="A56">
-        <v>53.0</v>
-      </c>
-    </row>
-    <row r="57" ht="14.25" customHeight="1">
-      <c r="A57">
-        <v>54.0</v>
-      </c>
-    </row>
-    <row r="58" ht="14.25" customHeight="1">
-      <c r="A58">
-        <v>55.0</v>
-      </c>
-    </row>
-    <row r="59" ht="14.25" customHeight="1">
-      <c r="A59">
-        <v>56.0</v>
-      </c>
-    </row>
-    <row r="60" ht="14.25" customHeight="1">
-      <c r="A60">
-        <v>57.0</v>
-      </c>
-    </row>
-    <row r="61" ht="14.25" customHeight="1">
-      <c r="A61">
-        <v>58.0</v>
-      </c>
-    </row>
-    <row r="62" ht="14.25" customHeight="1">
-      <c r="A62">
-        <v>59.0</v>
-      </c>
-    </row>
-    <row r="63" ht="14.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A43" s="9">
+        <v>40</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A44" s="9">
+        <v>41</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A45" s="9">
+        <v>42</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="9">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A46" s="9">
+        <v>43</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="9">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A47" s="9">
+        <v>44</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="9">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A48" s="9">
+        <v>45</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="9">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A49" s="9">
+        <v>46</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="9">
+        <v>258.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A50" s="9">
+        <v>47</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="9">
+        <v>1.2857000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A51" s="9">
+        <v>48</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="9">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A52" s="9">
+        <v>49</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="9">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A53" s="9">
+        <v>50</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="9">
+        <v>649.71400000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A54" s="9">
+        <v>51</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" s="9">
+        <v>4981</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A55" s="9">
+        <v>52</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="9">
+        <v>9798</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A56" s="9">
+        <v>53</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="9">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A57" s="9">
+        <v>54</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="9">
+        <v>5922</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A58" s="9">
+        <v>55</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A59" s="9">
+        <v>56</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="9">
+        <v>307.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A60" s="9">
+        <v>57</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A61" s="9">
+        <v>58</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A62" s="9">
+        <v>59</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1">
       <c r="A63" s="3">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C63" s="3">
-        <v>-927.4285714</v>
-      </c>
-    </row>
-    <row r="64" ht="14.25" customHeight="1">
+        <v>-927.42857140000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1">
       <c r="A64" s="3">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C64" s="3">
-        <v>123.0</v>
-      </c>
-    </row>
-    <row r="65" ht="14.25" customHeight="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="14.25" customHeight="1">
       <c r="A65" s="3">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>47</v>
@@ -896,20 +1390,20 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="66" ht="14.25" customHeight="1">
+    <row r="66" spans="1:3" ht="14.25" customHeight="1">
       <c r="A66" s="3">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="3">
-        <v>81.85714286</v>
-      </c>
-    </row>
-    <row r="67" ht="14.25" customHeight="1">
+        <v>81.857142859999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="14.25" customHeight="1">
       <c r="A67" s="3">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>49</v>
@@ -918,20 +1412,20 @@
         <v>702.92</v>
       </c>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
+    <row r="68" spans="1:3" ht="14.25" customHeight="1">
       <c r="A68" s="3">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C68" s="3">
-        <v>-631.2676056</v>
-      </c>
-    </row>
-    <row r="69" ht="14.25" customHeight="1">
+        <v>-631.26760560000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="14.25" customHeight="1">
       <c r="A69" s="3">
-        <v>66.0</v>
+        <v>66</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>51</v>
@@ -940,20 +1434,20 @@
         <v>121.5</v>
       </c>
     </row>
-    <row r="70" ht="14.25" customHeight="1">
+    <row r="70" spans="1:3" ht="14.25" customHeight="1">
       <c r="A70" s="3">
-        <v>67.0</v>
+        <v>67</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C70" s="3">
-        <v>0.714285714</v>
-      </c>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
+        <v>0.71428571399999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="14.25" customHeight="1">
       <c r="A71" s="3">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>53</v>
@@ -962,237 +1456,237 @@
         <v>20.125</v>
       </c>
     </row>
-    <row r="72" ht="14.25" customHeight="1">
+    <row r="72" spans="1:3" ht="14.25" customHeight="1">
       <c r="A72" s="3">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C72" s="3">
-        <v>132.0</v>
-      </c>
-    </row>
-    <row r="73" ht="14.25" customHeight="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="14.25" customHeight="1">
       <c r="A73" s="3">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C73" s="3">
-        <v>990.0</v>
-      </c>
-    </row>
-    <row r="74" ht="14.25" customHeight="1">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="14.25" customHeight="1">
       <c r="A74" s="3">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C74" s="3">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="75" ht="14.25" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="14.25" customHeight="1">
       <c r="A75" s="3">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C75" s="3">
-        <v>9000.0</v>
-      </c>
-    </row>
-    <row r="76" ht="14.25" customHeight="1">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="14.25" customHeight="1">
       <c r="A76" s="3">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C76" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="77" ht="14.25" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="14.25" customHeight="1">
       <c r="A77" s="3">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="B77" s="7">
-        <v>42742.0</v>
+        <v>42742</v>
       </c>
       <c r="C77" s="3">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="78" ht="14.25" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="14.25" customHeight="1">
       <c r="A78" s="3">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C78" s="3">
-        <v>4.333333333</v>
-      </c>
-    </row>
-    <row r="79" ht="14.25" customHeight="1">
+        <v>4.3333333329999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="14.25" customHeight="1">
       <c r="A79" s="3">
-        <v>76.0</v>
+        <v>76</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C79" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="80" ht="14.25" customHeight="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="14.25" customHeight="1">
       <c r="A80" s="3">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C80" s="3">
-        <v>48.0</v>
-      </c>
-    </row>
-    <row r="81" ht="14.25" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="14.25" customHeight="1">
       <c r="A81" s="3">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C81" s="3">
-        <v>258.0</v>
-      </c>
-    </row>
-    <row r="82" ht="14.25" customHeight="1">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="14.25" customHeight="1">
       <c r="A82" s="3">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C82" s="8">
-        <v>1.59814E14</v>
-      </c>
-    </row>
-    <row r="83" ht="14.25" customHeight="1">
+        <v>159814000000000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="14.25" customHeight="1">
       <c r="A83">
-        <v>80.0</v>
-      </c>
-    </row>
-    <row r="84" ht="14.25" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="14.25" customHeight="1">
       <c r="A84">
-        <v>81.0</v>
-      </c>
-    </row>
-    <row r="85" ht="14.25" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="14.25" customHeight="1">
       <c r="A85">
-        <v>82.0</v>
-      </c>
-    </row>
-    <row r="86" ht="14.25" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="14.25" customHeight="1">
       <c r="A86">
-        <v>83.0</v>
-      </c>
-    </row>
-    <row r="87" ht="14.25" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="14.25" customHeight="1">
       <c r="A87">
-        <v>84.0</v>
-      </c>
-    </row>
-    <row r="88" ht="14.25" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="14.25" customHeight="1">
       <c r="A88">
-        <v>85.0</v>
-      </c>
-    </row>
-    <row r="89" ht="14.25" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="14.25" customHeight="1">
       <c r="A89">
-        <v>86.0</v>
-      </c>
-    </row>
-    <row r="90" ht="14.25" customHeight="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="14.25" customHeight="1">
       <c r="A90">
-        <v>87.0</v>
-      </c>
-    </row>
-    <row r="91" ht="14.25" customHeight="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="14.25" customHeight="1">
       <c r="A91">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="92" ht="14.25" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="14.25" customHeight="1">
       <c r="A92">
-        <v>89.0</v>
-      </c>
-    </row>
-    <row r="93" ht="14.25" customHeight="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="14.25" customHeight="1">
       <c r="A93">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="94" ht="14.25" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="14.25" customHeight="1">
       <c r="A94">
-        <v>91.0</v>
-      </c>
-    </row>
-    <row r="95" ht="14.25" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="14.25" customHeight="1">
       <c r="A95">
-        <v>92.0</v>
-      </c>
-    </row>
-    <row r="96" ht="14.25" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="14.25" customHeight="1">
       <c r="A96">
-        <v>93.0</v>
-      </c>
-    </row>
-    <row r="97" ht="14.25" customHeight="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="14.25" customHeight="1">
       <c r="A97">
-        <v>94.0</v>
-      </c>
-    </row>
-    <row r="98" ht="14.25" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="14.25" customHeight="1">
       <c r="A98">
-        <v>95.0</v>
-      </c>
-    </row>
-    <row r="99" ht="14.25" customHeight="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="14.25" customHeight="1">
       <c r="A99">
-        <v>96.0</v>
-      </c>
-    </row>
-    <row r="100" ht="14.25" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="14.25" customHeight="1">
       <c r="A100">
-        <v>97.0</v>
-      </c>
-    </row>
-    <row r="101" ht="14.25" customHeight="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="14.25" customHeight="1">
       <c r="A101">
-        <v>98.0</v>
-      </c>
-    </row>
-    <row r="102" ht="14.25" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="14.25" customHeight="1">
       <c r="A102">
-        <v>99.0</v>
-      </c>
-    </row>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="104" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="105" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="106" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="107" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="108" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="109" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="110" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="111" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="112" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="113" ht="14.25" customHeight="1"/>
     <row r="114" ht="14.25" customHeight="1"/>
     <row r="115" ht="14.25" customHeight="1"/>
@@ -2083,20 +2577,22 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D3"/>
+    <hyperlink ref="D3" r:id="rId1"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="9.38"/>
+    <col min="1" max="26" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -3100,18 +3596,19 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="9.38"/>
+    <col min="1" max="26" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -4115,6 +4612,6 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted Equalssign in image_numbers, deleted placeholder image for GUI
</commit_message>
<xml_diff>
--- a/code/testset/image_numbers.xlsx
+++ b/code/testset/image_numbers.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Björn\Uni\WS17\EDBV\edbv\code\testset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktoria\Documents\edbv\code\testset\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="225" yWindow="570" windowWidth="13110" windowHeight="3390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="570" windowWidth="13110" windowHeight="3390"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -155,45 +155,12 @@
     <t>22*(9/3)-25</t>
   </si>
   <si>
-    <t>(99+1)/((1+3)*7)-(133*7)=</t>
-  </si>
-  <si>
-    <t>((17*3)-10)*3=</t>
-  </si>
-  <si>
-    <t>(3+77-7)/2=</t>
-  </si>
-  <si>
     <t>((5+8+178)*3)/7</t>
   </si>
   <si>
-    <t>(538/50)*17+631-111=</t>
-  </si>
-  <si>
-    <t>(11*321)/71-681=</t>
-  </si>
-  <si>
-    <t>6*(78+3)/4=</t>
-  </si>
-  <si>
-    <t>96/7-13=</t>
-  </si>
-  <si>
-    <t>11+730/80=</t>
-  </si>
-  <si>
-    <t>(10+23)*4 =</t>
-  </si>
-  <si>
     <t>(88-47+3)*45/2</t>
   </si>
   <si>
-    <t>4*5+8 =</t>
-  </si>
-  <si>
-    <t>(999*9)+9 =</t>
-  </si>
-  <si>
     <t>1/1-(1*1)+1</t>
   </si>
   <si>
@@ -348,12 +315,45 @@
   </si>
   <si>
     <t>-8*(3/1)+2</t>
+  </si>
+  <si>
+    <t>(99+1)/((1+3)*7)-(133*7)</t>
+  </si>
+  <si>
+    <t>((17*3)-10)*3</t>
+  </si>
+  <si>
+    <t>(3+77-7)/2</t>
+  </si>
+  <si>
+    <t>(538/50)*17+631-111</t>
+  </si>
+  <si>
+    <t>(11*321)/71-681</t>
+  </si>
+  <si>
+    <t>6*(78+3)/4</t>
+  </si>
+  <si>
+    <t>96/7-13</t>
+  </si>
+  <si>
+    <t>11+730/80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(10+23)*4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(999*9)+9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4*5+8 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -457,7 +457,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -532,23 +532,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -584,23 +567,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -776,17 +742,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
@@ -811,19 +777,19 @@
         <v>3</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1">
@@ -1272,7 +1238,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C43" s="8">
         <v>12</v>
@@ -1283,7 +1249,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C44" s="8">
         <v>41</v>
@@ -1294,7 +1260,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C45" s="8">
         <v>82.5</v>
@@ -1305,7 +1271,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C46" s="8">
         <v>460</v>
@@ -1316,7 +1282,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C47" s="8">
         <v>1300</v>
@@ -1327,7 +1293,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C48" s="8">
         <v>684</v>
@@ -1338,7 +1304,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C49" s="8">
         <v>258.5</v>
@@ -1349,7 +1315,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C50" s="8">
         <v>1.2857000000000001</v>
@@ -1360,7 +1326,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C51" s="8">
         <v>1360</v>
@@ -1371,7 +1337,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C52" s="8">
         <v>260</v>
@@ -1382,7 +1348,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C53" s="8">
         <v>649.71400000000006</v>
@@ -1393,7 +1359,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C54" s="8">
         <v>4981</v>
@@ -1404,7 +1370,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C55" s="8">
         <v>9798</v>
@@ -1415,7 +1381,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C56" s="8">
         <v>333</v>
@@ -1426,7 +1392,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C57" s="8">
         <v>5922</v>
@@ -1437,7 +1403,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C58" s="8">
         <v>10</v>
@@ -1448,7 +1414,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C59" s="8">
         <v>307.5</v>
@@ -1459,7 +1425,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C60" s="8">
         <v>54</v>
@@ -1470,7 +1436,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C61" s="8">
         <v>16</v>
@@ -1481,7 +1447,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C62" s="8">
         <v>0</v>
@@ -1492,7 +1458,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="C63" s="3">
         <v>-927.42857140000001</v>
@@ -1503,7 +1469,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C64" s="3">
         <v>123</v>
@@ -1514,7 +1480,7 @@
         <v>62</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="C65" s="3">
         <v>36.5</v>
@@ -1525,7 +1491,7 @@
         <v>63</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C66" s="3">
         <v>81.857142859999996</v>
@@ -1536,7 +1502,7 @@
         <v>64</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="C67" s="3">
         <v>702.92</v>
@@ -1547,7 +1513,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="C68" s="3">
         <v>-631.26760560000002</v>
@@ -1558,7 +1524,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="C69" s="3">
         <v>121.5</v>
@@ -1569,7 +1535,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="C70" s="3">
         <v>0.71428571399999996</v>
@@ -1580,7 +1546,7 @@
         <v>68</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="C71" s="3">
         <v>20.125</v>
@@ -1591,7 +1557,7 @@
         <v>69</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="C72" s="3">
         <v>132</v>
@@ -1602,7 +1568,7 @@
         <v>70</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C73" s="3">
         <v>990</v>
@@ -1613,7 +1579,7 @@
         <v>71</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="C74" s="3">
         <v>28</v>
@@ -1624,7 +1590,7 @@
         <v>72</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="C75" s="3">
         <v>9000</v>
@@ -1635,7 +1601,7 @@
         <v>73</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C76" s="3">
         <v>1</v>
@@ -1646,7 +1612,7 @@
         <v>74</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C77" s="3">
         <v>7</v>
@@ -1657,7 +1623,7 @@
         <v>75</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C78" s="3">
         <v>4.3333333329999997</v>
@@ -1668,7 +1634,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C79" s="3">
         <v>0</v>
@@ -1679,7 +1645,7 @@
         <v>77</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C80" s="3">
         <v>48</v>
@@ -1690,7 +1656,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C81" s="3">
         <v>258</v>
@@ -1701,7 +1667,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C82" s="7">
         <v>159814000000000</v>
@@ -1712,7 +1678,7 @@
         <v>80</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C83" s="6">
         <v>6</v>
@@ -1723,7 +1689,7 @@
         <v>81</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C84" s="6">
         <v>-22</v>
@@ -1734,7 +1700,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C85" s="6">
         <v>666.63333299999999</v>
@@ -1745,7 +1711,7 @@
         <v>83</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C86" s="6">
         <v>-1.1785714300000001</v>
@@ -1756,7 +1722,7 @@
         <v>84</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C87" s="6">
         <v>6342</v>
@@ -1767,7 +1733,7 @@
         <v>85</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C88" s="6">
         <v>24</v>
@@ -1778,7 +1744,7 @@
         <v>86</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C89" s="6">
         <v>3.5757575799999999</v>
@@ -1789,7 +1755,7 @@
         <v>87</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C90" s="6">
         <v>-7364</v>
@@ -1800,7 +1766,7 @@
         <v>88</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C91" s="6">
         <v>0.38888888999999999</v>
@@ -1811,7 +1777,7 @@
         <v>89</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C92" s="6">
         <v>2600</v>
@@ -1822,7 +1788,7 @@
         <v>90</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C93" s="6">
         <v>350</v>
@@ -1833,7 +1799,7 @@
         <v>91</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C94" s="6">
         <v>14</v>
@@ -1844,7 +1810,7 @@
         <v>92</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C95" s="6">
         <v>9</v>
@@ -1855,7 +1821,7 @@
         <v>93</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C96" s="6">
         <v>0.24</v>
@@ -1866,7 +1832,7 @@
         <v>94</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C97" s="6">
         <v>-33</v>
@@ -1877,7 +1843,7 @@
         <v>95</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C98" s="6">
         <v>71</v>
@@ -1888,7 +1854,7 @@
         <v>96</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C99" s="6">
         <v>20.578947400000001</v>
@@ -1899,7 +1865,7 @@
         <v>97</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C100" s="6">
         <v>14.0384615</v>
@@ -1910,7 +1876,7 @@
         <v>98</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C101" s="6">
         <v>-236</v>
@@ -1921,7 +1887,7 @@
         <v>99</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C102" s="6">
         <v>3</v>
@@ -2832,7 +2798,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3848,7 +3814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>